<commit_message>
part of General page I
</commit_message>
<xml_diff>
--- a/src/test/test_data/polovniautomobili.xlsx
+++ b/src/test/test_data/polovniautomobili.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\polovniAutomobili\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AD0385-75DA-4E32-BA4C-1805390C456A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7AECD6-5C8C-48E9-8913-49A986BC8910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">login!$A$3:$B$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="212">
   <si>
     <t>tc_id</t>
   </si>
@@ -649,6 +650,24 @@
   </si>
   <si>
     <t>SI_018</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Najnoviji oglasi</t>
+  </si>
+  <si>
+    <t>FORTH</t>
+  </si>
+  <si>
+    <t>Postavi oglas</t>
+  </si>
+  <si>
+    <t>Prodaj sopstveno vozilo</t>
+  </si>
+  <si>
+    <t>Oglasi celokupnu ponudu</t>
+  </si>
+  <si>
+    <t>Ubrzaj prodaju</t>
   </si>
 </sst>
 </file>
@@ -4337,7 +4356,7 @@
   <dimension ref="A1:AH21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4505,7 +4524,9 @@
       <c r="G4" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="11" t="s">
+        <v>206</v>
+      </c>
       <c r="I4" s="11" t="s">
         <v>144</v>
       </c>
@@ -4747,20 +4768,32 @@
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="11" t="s">
+        <v>207</v>
+      </c>
       <c r="E8" s="11" t="s">
         <v>161</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="G8" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>

</xml_diff>

<commit_message>
login page is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/polovniautomobili.xlsx
+++ b/src/test/test_data/polovniautomobili.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\polovniAutomobili\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7AECD6-5C8C-48E9-8913-49A986BC8910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3A611E-53BF-4944-8D69-316D06031914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="women" sheetId="2" r:id="rId2"/>
+    <sheet name="automobili" sheetId="1" r:id="rId1"/>
+    <sheet name="mojprofil" sheetId="2" r:id="rId2"/>
     <sheet name="men" sheetId="3" r:id="rId3"/>
     <sheet name="general" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">login!$A$3:$B$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">automobili!$A$3:$B$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="228">
   <si>
     <t>tc_id</t>
   </si>
@@ -52,15 +51,9 @@
     <t>SI_004</t>
   </si>
   <si>
-    <t>urlBasePage</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
-    <t>testType</t>
-  </si>
-  <si>
     <t>attributeType</t>
   </si>
   <si>
@@ -82,42 +75,15 @@
     <t>no</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>SI_007</t>
   </si>
   <si>
     <t>SI_008</t>
   </si>
   <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
-    <t>sasa</t>
-  </si>
-  <si>
-    <t>stjepanovic</t>
-  </si>
-  <si>
-    <t>stjepanovic1@yahoo.com</t>
-  </si>
-  <si>
-    <t>Stjepanovic@12</t>
-  </si>
-  <si>
-    <t>confirmPassword</t>
-  </si>
-  <si>
-    <t>Test import data for "Magneto" project</t>
-  </si>
-  <si>
     <t>accountRegistered</t>
   </si>
   <si>
@@ -130,9 +96,6 @@
     <t>This is a required field.</t>
   </si>
   <si>
-    <t>field</t>
-  </si>
-  <si>
     <t>firstname</t>
   </si>
   <si>
@@ -145,9 +108,6 @@
     <t>confirmpassword</t>
   </si>
   <si>
-    <t>stjepanovic1</t>
-  </si>
-  <si>
     <t>Please enter a valid email address (Ex: johndoe@domain.com).</t>
   </si>
   <si>
@@ -169,9 +129,6 @@
     <t>SI_015</t>
   </si>
   <si>
-    <t>stjepa</t>
-  </si>
-  <si>
     <t>Password Strength: No Password</t>
   </si>
   <si>
@@ -184,21 +141,12 @@
     <t>strengthpassword</t>
   </si>
   <si>
-    <t>Kikinda1</t>
-  </si>
-  <si>
     <t>Password Strength: Medium</t>
   </si>
   <si>
-    <t>Stjepanovic</t>
-  </si>
-  <si>
     <t>Please enter the same value again.</t>
   </si>
   <si>
-    <t>wrong</t>
-  </si>
-  <si>
     <t>both</t>
   </si>
   <si>
@@ -220,21 +168,12 @@
     <t>Men</t>
   </si>
   <si>
-    <t>What's New</t>
-  </si>
-  <si>
-    <t>Women</t>
-  </si>
-  <si>
     <t>Gear</t>
   </si>
   <si>
     <t>Training</t>
   </si>
   <si>
-    <t>Sale</t>
-  </si>
-  <si>
     <t>menuItemTitle1</t>
   </si>
   <si>
@@ -250,12 +189,6 @@
     <t>BOTTOMS</t>
   </si>
   <si>
-    <t>NEW IN WOMEN'S</t>
-  </si>
-  <si>
-    <t>NEW IN MEN'S</t>
-  </si>
-  <si>
     <t>product</t>
   </si>
   <si>
@@ -286,15 +219,9 @@
     <t>productType</t>
   </si>
   <si>
-    <t>women</t>
-  </si>
-  <si>
     <t>Tanks</t>
   </si>
   <si>
-    <t>men</t>
-  </si>
-  <si>
     <t>h</t>
   </si>
   <si>
@@ -379,9 +306,6 @@
     <t>categoryItemWomen1</t>
   </si>
   <si>
-    <t>Capri</t>
-  </si>
-  <si>
     <t>categoryMen1</t>
   </si>
   <si>
@@ -415,12 +339,6 @@
     <t>searchRowNumber2</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>ulrPage</t>
   </si>
   <si>
@@ -668,6 +586,135 @@
   </si>
   <si>
     <t>Ubrzaj prodaju</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>marka</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>cenaDo</t>
+  </si>
+  <si>
+    <t>godisteOd</t>
+  </si>
+  <si>
+    <t>godisteDo</t>
+  </si>
+  <si>
+    <t>karoserija</t>
+  </si>
+  <si>
+    <t>gorivo</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>polovna_nova_vozila</t>
+  </si>
+  <si>
+    <t>pretraga</t>
+  </si>
+  <si>
+    <t>kredit</t>
+  </si>
+  <si>
+    <t>lizing</t>
+  </si>
+  <si>
+    <t>garancija</t>
+  </si>
+  <si>
+    <t>najnovijiOglasi</t>
+  </si>
+  <si>
+    <t>Automobili</t>
+  </si>
+  <si>
+    <t>Asia Motors</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>subItem1</t>
+  </si>
+  <si>
+    <t>subItem2</t>
+  </si>
+  <si>
+    <t>subItem3</t>
+  </si>
+  <si>
+    <t>subItem4</t>
+  </si>
+  <si>
+    <t>subItem5</t>
+  </si>
+  <si>
+    <t>subItem6</t>
+  </si>
+  <si>
+    <t>subItem7</t>
+  </si>
+  <si>
+    <t>subItem8</t>
+  </si>
+  <si>
+    <t>subItem9</t>
+  </si>
+  <si>
+    <t>subItem10a</t>
+  </si>
+  <si>
+    <t>subItem10b</t>
+  </si>
+  <si>
+    <t>Prijavi se</t>
+  </si>
+  <si>
+    <t>stjepanovic11temp@gmail.com</t>
+  </si>
+  <si>
+    <t>stjepatemp</t>
+  </si>
+  <si>
+    <t>verificationType</t>
+  </si>
+  <si>
+    <t>goodCredentials</t>
+  </si>
+  <si>
+    <t>wrongEmail</t>
+  </si>
+  <si>
+    <t>rightEmailEnteredYesNo</t>
+  </si>
+  <si>
+    <t>xxyyyxxxyyy</t>
+  </si>
+  <si>
+    <t>wrongPassword</t>
+  </si>
+  <si>
+    <t>verificationText</t>
+  </si>
+  <si>
+    <t>Ne postoji nalog sa ovom mail adresom.</t>
+  </si>
+  <si>
+    <t>Proveri da li si dobro uneo e-mail i/ili šifru.</t>
+  </si>
+  <si>
+    <t>xxxxyyyxx</t>
+  </si>
+  <si>
+    <t>Krediti</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1273,7 @@
   <dimension ref="A1:W18"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,19 +1281,19 @@
     <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="1" customWidth="1"/>
-    <col min="11" max="11" width="29.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="29.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" style="1" customWidth="1"/>
     <col min="17" max="17" width="15.5703125" style="1" customWidth="1"/>
     <col min="18" max="18" width="21.85546875" style="1" customWidth="1"/>
     <col min="19" max="19" width="15.5703125" style="1" customWidth="1"/>
@@ -1258,7 +1305,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -1292,792 +1339,450 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>19</v>
+        <v>185</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>21</v>
+        <v>187</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>7</v>
+        <v>188</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>26</v>
+        <v>189</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>8</v>
+        <v>190</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>14</v>
+        <v>191</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>28</v>
+        <v>192</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>9</v>
+        <v>193</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>30</v>
+        <v>194</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>32</v>
+        <v>197</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>6</v>
+        <v>198</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>82</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
     </row>
     <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>22</v>
+      <c r="B4" s="11" t="s">
+        <v>200</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>25</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="11"/>
-      <c r="H4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>31</v>
-      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
       <c r="L4" s="11"/>
-      <c r="M4" s="11" t="s">
-        <v>60</v>
-      </c>
+      <c r="M4" s="11"/>
       <c r="N4" s="11"/>
       <c r="O4" s="11"/>
-      <c r="P4" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="U4" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="V4" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
+      <c r="C5" s="11" t="s">
+        <v>202</v>
+      </c>
       <c r="D5" s="11"/>
-      <c r="E5" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>25</v>
-      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
       <c r="G5" s="11"/>
-      <c r="H5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>31</v>
-      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
-      <c r="N5" s="11" t="s">
-        <v>21</v>
-      </c>
+      <c r="N5" s="11"/>
       <c r="O5" s="11"/>
-      <c r="P5" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>25</v>
-      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
-      <c r="K6" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="11" t="s">
-        <v>33</v>
-      </c>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
       <c r="O6" s="11"/>
-      <c r="P6" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="R6" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="S6" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="T6" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="U6" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="V6" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="B7" s="10"/>
       <c r="C7" s="11"/>
-      <c r="D7" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>25</v>
-      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="11" t="s">
-        <v>34</v>
-      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
       <c r="O7" s="11"/>
-      <c r="P7" s="11" t="s">
-        <v>64</v>
-      </c>
+      <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
-      <c r="R7" s="11" t="s">
-        <v>77</v>
-      </c>
+      <c r="R7" s="11"/>
       <c r="S7" s="11"/>
-      <c r="T7" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="U7" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="V7" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="S8" s="15"/>
-      <c r="T8" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="U8" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="V8" s="11" t="s">
-        <v>15</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17" t="s">
-        <v>25</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="11"/>
-      <c r="H9" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
-      <c r="K9" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="11" t="s">
-        <v>7</v>
-      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
       <c r="O9" s="11"/>
-      <c r="P9" s="11" t="s">
-        <v>66</v>
-      </c>
+      <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
-      <c r="R9" s="15" t="s">
-        <v>79</v>
-      </c>
+      <c r="R9" s="11"/>
       <c r="S9" s="11"/>
-      <c r="T9" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="U9" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="V9" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="17"/>
+        <v>14</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="S10" s="6"/>
-      <c r="T10" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="U10" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="V10" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>25</v>
-      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="U11" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="V11" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="U12" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="V12" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="U13" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="V13" s="11" t="s">
-        <v>15</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>25</v>
-      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="U14" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="V14" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B15" s="10"/>
-      <c r="C15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>25</v>
-      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="U15" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="V15" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>25</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="U16" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="V16" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>25</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="L17" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
       <c r="M17" s="11"/>
-      <c r="N17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
@@ -2095,10 +1800,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD393A5-6731-4B8E-BE1C-8BAF208C9B9B}">
-  <dimension ref="A1:AI20"/>
+  <dimension ref="A1:AJ20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,38 +1811,40 @@
     <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="21" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="21" style="1" customWidth="1"/>
-    <col min="19" max="19" width="24" style="1" customWidth="1"/>
-    <col min="20" max="20" width="20" style="1" customWidth="1"/>
-    <col min="21" max="22" width="17.42578125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="24" style="1" customWidth="1"/>
-    <col min="24" max="25" width="21.5703125" style="1" customWidth="1"/>
-    <col min="26" max="27" width="19.140625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="19.42578125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="19.5703125" style="1" customWidth="1"/>
-    <col min="30" max="31" width="19.140625" style="1" customWidth="1"/>
-    <col min="32" max="32" width="17" style="1" customWidth="1"/>
-    <col min="33" max="33" width="15.7109375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="14.42578125" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="23.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="21" style="1" customWidth="1"/>
+    <col min="20" max="20" width="24" style="1" customWidth="1"/>
+    <col min="21" max="21" width="20" style="1" customWidth="1"/>
+    <col min="22" max="23" width="17.42578125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="24" style="1" customWidth="1"/>
+    <col min="25" max="26" width="21.5703125" style="1" customWidth="1"/>
+    <col min="27" max="28" width="19.140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="19.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="19.5703125" style="1" customWidth="1"/>
+    <col min="31" max="32" width="19.140625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="17" style="1" customWidth="1"/>
+    <col min="34" max="34" width="15.7109375" style="1" customWidth="1"/>
+    <col min="35" max="35" width="14.42578125" style="1" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -2172,116 +1879,120 @@
       <c r="AF1" s="27"/>
       <c r="AG1" s="27"/>
       <c r="AH1" s="27"/>
-    </row>
-    <row r="2" spans="1:34" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI1" s="27"/>
+    </row>
+    <row r="2" spans="1:35" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
       <c r="B2" s="23"/>
     </row>
-    <row r="3" spans="1:34" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>203</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>20</v>
+        <v>204</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>7</v>
+        <v>206</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>26</v>
+        <v>207</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>14</v>
+        <v>209</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>28</v>
+        <v>210</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>9</v>
+        <v>211</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>30</v>
+        <v>212</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>57</v>
+        <v>213</v>
       </c>
       <c r="M3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="S3" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="U3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="V3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="X3" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Y3" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z3" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="Q3" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="R3" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="W3" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="X3" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y3" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z3" s="7" t="s">
-        <v>121</v>
-      </c>
       <c r="AA3" s="7" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="AB3" s="7" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="AC3" s="7" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="AD3" s="7" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="AE3" s="7" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="AF3" s="7" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="AG3" s="7" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="AH3" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2291,73 +2002,48 @@
       <c r="E4" s="11"/>
       <c r="F4" s="17"/>
       <c r="G4" s="11"/>
-      <c r="H4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
       <c r="K4" s="11" t="s">
-        <v>31</v>
+        <v>214</v>
       </c>
       <c r="L4" s="11"/>
       <c r="M4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="N4" s="11"/>
+        <v>215</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>216</v>
+      </c>
       <c r="O4" s="11" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>90</v>
+        <v>218</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="U4" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="V4" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="W4" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="X4" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y4" s="11" t="s">
-        <v>99</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
       <c r="Z4" s="11"/>
       <c r="AA4" s="11"/>
       <c r="AB4" s="11"/>
       <c r="AC4" s="11"/>
       <c r="AD4" s="11"/>
       <c r="AE4" s="11"/>
-      <c r="AF4" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG4" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH4" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="11"/>
+      <c r="AI4" s="11"/>
+    </row>
+    <row r="5" spans="1:35" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2367,73 +2053,44 @@
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="11"/>
-      <c r="H5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
       <c r="K5" s="11" t="s">
-        <v>31</v>
+        <v>227</v>
       </c>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
-      <c r="N5" s="11" t="s">
-        <v>21</v>
-      </c>
+      <c r="N5" s="11"/>
       <c r="O5" s="15" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="P5" s="15" t="s">
-        <v>90</v>
+        <v>219</v>
       </c>
       <c r="Q5" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="W5" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="X5" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y5" s="11" t="s">
-        <v>103</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="R5" s="15"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="11"/>
       <c r="Z5" s="11"/>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11"/>
       <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
       <c r="AE5" s="11"/>
-      <c r="AF5" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG5" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH5" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="11"/>
+      <c r="AH5" s="11"/>
+      <c r="AI5" s="11"/>
+    </row>
+    <row r="6" spans="1:35" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2443,81 +2100,44 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
-      <c r="K6" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="K6" s="13"/>
       <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="11" t="s">
-        <v>33</v>
-      </c>
+      <c r="M6" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="N6" s="11"/>
       <c r="O6" s="15" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>92</v>
+        <v>219</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="R6" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="S6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="T6" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="U6" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="V6" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="W6" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="X6" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y6" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA6" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB6" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC6" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="AD6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF6" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH6" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+      <c r="R6" s="15"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="15"/>
+      <c r="AE6" s="15"/>
+      <c r="AF6" s="15"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
+    </row>
+    <row r="7" spans="1:35" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2527,67 +2147,46 @@
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="K7" s="13"/>
       <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="11" t="s">
-        <v>34</v>
-      </c>
+      <c r="M7" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="N7" s="11"/>
       <c r="O7" s="15" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="P7" s="15" t="s">
-        <v>90</v>
+        <v>222</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="R7" s="11" t="s">
-        <v>63</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="R7" s="15"/>
       <c r="S7" s="11"/>
-      <c r="T7" s="11" t="s">
-        <v>77</v>
-      </c>
+      <c r="T7" s="11"/>
       <c r="U7" s="11"/>
-      <c r="V7" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="W7" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="X7" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y7" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="11"/>
       <c r="Z7" s="11"/>
       <c r="AA7" s="11"/>
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
       <c r="AD7" s="11"/>
       <c r="AE7" s="11"/>
-      <c r="AF7" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG7" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH7" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AF7" s="11"/>
+      <c r="AG7" s="11"/>
+      <c r="AH7" s="11"/>
+      <c r="AI7" s="11"/>
+    </row>
+    <row r="8" spans="1:35" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
@@ -2595,67 +2194,48 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15" t="s">
-        <v>15</v>
-      </c>
+      <c r="H8" s="15"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
-      <c r="K8" s="15" t="s">
-        <v>31</v>
-      </c>
+      <c r="K8" s="15"/>
       <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
+      <c r="M8" s="11" t="s">
+        <v>215</v>
+      </c>
       <c r="N8" s="15" t="s">
-        <v>21</v>
+        <v>226</v>
       </c>
       <c r="O8" s="15" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="P8" s="15" t="s">
-        <v>90</v>
+        <v>222</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="R8" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="S8" s="15"/>
-      <c r="T8" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="W8" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="X8" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y8" s="15" t="s">
-        <v>110</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="R8" s="15"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
       <c r="Z8" s="15"/>
       <c r="AA8" s="15"/>
       <c r="AB8" s="15"/>
       <c r="AC8" s="15"/>
       <c r="AD8" s="15"/>
       <c r="AE8" s="15"/>
-      <c r="AF8" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AG8" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH8" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AF8" s="15"/>
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="11"/>
+      <c r="AI8" s="11"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
@@ -2663,67 +2243,38 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="11"/>
-      <c r="H9" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
-      <c r="K9" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
-      <c r="N9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="O9" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="P9" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q9" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="R9" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="N9" s="11"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
       <c r="S9" s="11"/>
-      <c r="T9" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="U9" s="11"/>
-      <c r="V9" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="W9" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="X9" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y9" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z9" s="15"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="11"/>
       <c r="AA9" s="15"/>
       <c r="AB9" s="15"/>
       <c r="AC9" s="15"/>
       <c r="AD9" s="15"/>
       <c r="AE9" s="15"/>
-      <c r="AF9" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG9" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH9" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AF9" s="15"/>
+      <c r="AG9" s="15"/>
+      <c r="AH9" s="11"/>
+      <c r="AI9" s="11"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
@@ -2731,36 +2282,20 @@
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H10" s="11"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="15" t="s">
-        <v>31</v>
-      </c>
+      <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
-      <c r="N10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="O10" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="P10" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q10" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="R10" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="S10" s="6"/>
-      <c r="T10" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="U10" s="6"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="11"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
@@ -2771,19 +2306,14 @@
       <c r="AC10" s="6"/>
       <c r="AD10" s="6"/>
       <c r="AE10" s="6"/>
-      <c r="AF10" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH10" s="11" t="s">
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="11"/>
+      <c r="AI10" s="11"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
@@ -2791,33 +2321,17 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
-      <c r="N11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="O11" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="P11" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q11" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="R11" s="6"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
@@ -2831,19 +2345,14 @@
       <c r="AC11" s="6"/>
       <c r="AD11" s="6"/>
       <c r="AE11" s="6"/>
-      <c r="AF11" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG11" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH11" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="11"/>
+      <c r="AH11" s="11"/>
+      <c r="AI11" s="11"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
@@ -2851,29 +2360,17 @@
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H12" s="11"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="15" t="s">
-        <v>46</v>
-      </c>
+      <c r="K12" s="15"/>
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
-      <c r="N12" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="O12" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="P12" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q12" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="R12" s="6"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
@@ -2887,19 +2384,14 @@
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="6"/>
-      <c r="AF12" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG12" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH12" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AF12" s="6"/>
+      <c r="AG12" s="11"/>
+      <c r="AH12" s="11"/>
+      <c r="AI12" s="11"/>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
@@ -2907,29 +2399,17 @@
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
-      <c r="H13" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H13" s="11"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="15" t="s">
-        <v>47</v>
-      </c>
+      <c r="K13" s="15"/>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
-      <c r="N13" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="O13" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="P13" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q13" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="R13" s="6"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
@@ -2943,19 +2423,14 @@
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
-      <c r="AF13" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG13" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH13" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AF13" s="6"/>
+      <c r="AG13" s="11"/>
+      <c r="AH13" s="11"/>
+      <c r="AI13" s="11"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
@@ -2963,29 +2438,17 @@
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H14" s="11"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="15" t="s">
-        <v>51</v>
-      </c>
+      <c r="K14" s="15"/>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
-      <c r="N14" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="O14" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="P14" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q14" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="R14" s="6"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
@@ -2999,19 +2462,14 @@
       <c r="AC14" s="6"/>
       <c r="AD14" s="6"/>
       <c r="AE14" s="6"/>
-      <c r="AF14" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG14" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH14" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="AF14" s="6"/>
+      <c r="AG14" s="11"/>
+      <c r="AH14" s="11"/>
+      <c r="AI14" s="11"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
@@ -3019,33 +2477,21 @@
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H15" s="11"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="15" t="s">
-        <v>48</v>
-      </c>
+      <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
-      <c r="N15" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="O15" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="P15" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q15" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="R15" s="6"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
-      <c r="V15" s="19"/>
+      <c r="V15" s="6"/>
       <c r="W15" s="19"/>
       <c r="X15" s="19"/>
       <c r="Y15" s="19"/>
@@ -3055,19 +2501,14 @@
       <c r="AC15" s="19"/>
       <c r="AD15" s="19"/>
       <c r="AE15" s="19"/>
-      <c r="AF15" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG15" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH15" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="AF15" s="19"/>
+      <c r="AG15" s="15"/>
+      <c r="AH15" s="11"/>
+      <c r="AI15" s="11"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
@@ -3075,29 +2516,17 @@
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H16" s="11"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="15" t="s">
-        <v>53</v>
-      </c>
+      <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
-      <c r="N16" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="O16" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="P16" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q16" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="R16" s="6"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
@@ -3111,19 +2540,14 @@
       <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
       <c r="AE16" s="6"/>
-      <c r="AF16" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG16" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH16" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:35" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="11"/>
+      <c r="AH16" s="11"/>
+      <c r="AI16" s="11"/>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
@@ -3131,35 +2555,17 @@
       <c r="E17" s="11"/>
       <c r="F17" s="17"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="L17" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
       <c r="M17" s="11"/>
-      <c r="N17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="O17" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="P17" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q17" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="R17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
@@ -3175,13 +2581,12 @@
       <c r="AE17" s="6"/>
       <c r="AF17" s="6"/>
       <c r="AG17" s="6"/>
-      <c r="AH17" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH17" s="6"/>
+      <c r="AI17" s="11"/>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -3196,16 +2601,10 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
-      <c r="O18" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="P18" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q18" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="R18" s="6"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
@@ -3221,14 +2620,13 @@
       <c r="AE18" s="6"/>
       <c r="AF18" s="6"/>
       <c r="AG18" s="6"/>
-      <c r="AH18" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI18" s="6"/>
-    </row>
-    <row r="19" spans="1:35" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH18" s="6"/>
+      <c r="AI18" s="11"/>
+      <c r="AJ18" s="6"/>
+    </row>
+    <row r="19" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
@@ -3236,44 +2634,20 @@
       <c r="E19" s="11"/>
       <c r="F19" s="17"/>
       <c r="G19" s="11"/>
-      <c r="H19" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>31</v>
-      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
       <c r="L19" s="11"/>
-      <c r="M19" s="11" t="s">
-        <v>60</v>
-      </c>
+      <c r="M19" s="11"/>
       <c r="N19" s="11"/>
-      <c r="O19" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P19" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q19" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="R19" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="S19" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="T19" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="U19" s="11" t="s">
-        <v>71</v>
-      </c>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
       <c r="X19" s="11"/>
@@ -3284,19 +2658,14 @@
       <c r="AC19" s="11"/>
       <c r="AD19" s="11"/>
       <c r="AE19" s="11"/>
-      <c r="AF19" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG19" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH19" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:35" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="AF19" s="11"/>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="11"/>
+      <c r="AI19" s="11"/>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
@@ -3304,33 +2673,21 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="11"/>
-      <c r="H20" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="H20" s="11"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="15" t="s">
-        <v>48</v>
-      </c>
+      <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
-      <c r="N20" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="O20" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="P20" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q20" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="R20" s="6"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
-      <c r="V20" s="19"/>
+      <c r="V20" s="6"/>
       <c r="W20" s="19"/>
       <c r="X20" s="19"/>
       <c r="Y20" s="19"/>
@@ -3340,20 +2697,15 @@
       <c r="AC20" s="19"/>
       <c r="AD20" s="19"/>
       <c r="AE20" s="19"/>
-      <c r="AF20" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG20" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH20" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="AF20" s="19"/>
+      <c r="AG20" s="15"/>
+      <c r="AH20" s="11"/>
+      <c r="AI20" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:AH1"/>
+    <mergeCell ref="A1:AI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3426,67 +2778,67 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="G3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="O3" s="8" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3494,63 +2846,63 @@
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="K4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="L4" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="N4" s="11" t="s">
+      <c r="Q4" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="S4" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="O4" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>99</v>
-      </c>
       <c r="T4" s="11" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="34.5" x14ac:dyDescent="0.25">
@@ -3558,63 +2910,63 @@
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="N5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="R5" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="O5" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q5" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>99</v>
-      </c>
       <c r="S5" s="11" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="V5" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3622,59 +2974,59 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="13" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="11" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="R6" s="15" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="V6" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -3682,201 +3034,201 @@
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="13" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="11" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="M7" s="11"/>
       <c r="N7" s="11" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="O7" s="11"/>
       <c r="P7" s="11" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="15" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="M8" s="15"/>
       <c r="N8" s="11" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="15" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="S8" s="15" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="T8" s="11" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="13" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="M9" s="11"/>
       <c r="N9" s="15" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="O9" s="11"/>
       <c r="P9" s="15" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="R9" s="15" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="T9" s="15" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="V9" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="15" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="11" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="11" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
@@ -3884,44 +3236,44 @@
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
       <c r="T10" s="11" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="V10" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="D11" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
@@ -3932,40 +3284,40 @@
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="11" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="V11" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="15" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
@@ -3976,40 +3328,40 @@
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="T12" s="11" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="V12" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="15" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
@@ -4020,40 +3372,40 @@
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
       <c r="T13" s="11" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="U13" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="V13" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
@@ -4064,40 +3416,40 @@
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
       <c r="T14" s="11" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="U14" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="V14" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="15" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
@@ -4108,40 +3460,40 @@
       <c r="R15" s="19"/>
       <c r="S15" s="19"/>
       <c r="T15" s="15" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="U15" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="V15" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="15" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
@@ -4152,46 +3504,46 @@
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
       <c r="T16" s="11" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="U16" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="V16" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="6" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
@@ -4204,12 +3556,12 @@
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
       <c r="V17" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -4219,13 +3571,13 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
@@ -4238,91 +3590,91 @@
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
       <c r="V18" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="W18" s="6"/>
     </row>
     <row r="19" spans="1:23" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="N19" s="11" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="O19" s="11" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
       <c r="T19" s="11" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="U19" s="11" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="V19" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="15" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
@@ -4333,13 +3685,13 @@
       <c r="R20" s="19"/>
       <c r="S20" s="19"/>
       <c r="T20" s="15" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="U20" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="V20" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -4356,7 +3708,7 @@
   <dimension ref="A1:AH21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4393,7 +3745,7 @@
   <sheetData>
     <row r="1" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -4437,55 +3789,55 @@
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>181</v>
-      </c>
       <c r="I3" s="9" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
@@ -4510,52 +3862,52 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="S4" s="11"/>
       <c r="T4" s="11"/>
@@ -4581,37 +3933,37 @@
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>180</v>
+        <v>153</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
@@ -4641,44 +3993,44 @@
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>191</v>
+        <v>164</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="R6" s="11"/>
       <c r="S6" s="11"/>
@@ -4705,44 +4057,44 @@
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11" t="s">
-        <v>194</v>
+        <v>167</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
@@ -4764,33 +4116,33 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>211</v>
+        <v>184</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
@@ -4818,16 +4170,16 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -4860,16 +4212,16 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -4902,16 +4254,16 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -4944,16 +4296,16 @@
     </row>
     <row r="12" spans="1:34" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
@@ -4986,7 +4338,7 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -5024,7 +4376,7 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -5062,7 +4414,7 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -5100,7 +4452,7 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -5138,7 +4490,7 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -5176,7 +4528,7 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -5214,7 +4566,7 @@
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -5252,7 +4604,7 @@
     </row>
     <row r="20" spans="1:34" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -5290,7 +4642,7 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>

</xml_diff>

<commit_message>
registration page is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/polovniautomobili.xlsx
+++ b/src/test/test_data/polovniautomobili.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\polovniAutomobili\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3A611E-53BF-4944-8D69-316D06031914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1947A78F-8462-4962-8EBB-2FA2B695D24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="automobili" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="235">
   <si>
     <t>tc_id</t>
   </si>
@@ -715,6 +715,27 @@
   </si>
   <si>
     <t>Krediti</t>
+  </si>
+  <si>
+    <t>randomEmailYesNo</t>
+  </si>
+  <si>
+    <t>secondPassword</t>
+  </si>
+  <si>
+    <t>Mosorinska92</t>
+  </si>
+  <si>
+    <t>buttonColor</t>
+  </si>
+  <si>
+    <t>background-color</t>
+  </si>
+  <si>
+    <t>rgba(255, 165, 0, 1)</t>
+  </si>
+  <si>
+    <t>cssType</t>
   </si>
 </sst>
 </file>
@@ -1800,10 +1821,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD393A5-6731-4B8E-BE1C-8BAF208C9B9B}">
-  <dimension ref="A1:AJ20"/>
+  <dimension ref="A1:AM20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AL12" sqref="AL12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,36 +1834,38 @@
     <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" style="1" customWidth="1"/>
     <col min="13" max="13" width="23.140625" style="1" customWidth="1"/>
     <col min="14" max="14" width="10.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="23.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="21" style="1" customWidth="1"/>
-    <col min="20" max="20" width="24" style="1" customWidth="1"/>
-    <col min="21" max="21" width="20" style="1" customWidth="1"/>
-    <col min="22" max="23" width="17.42578125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="24" style="1" customWidth="1"/>
-    <col min="25" max="26" width="21.5703125" style="1" customWidth="1"/>
-    <col min="27" max="28" width="19.140625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="19.42578125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="19.5703125" style="1" customWidth="1"/>
-    <col min="31" max="32" width="19.140625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="17" style="1" customWidth="1"/>
-    <col min="34" max="34" width="15.7109375" style="1" customWidth="1"/>
-    <col min="35" max="35" width="14.42578125" style="1" customWidth="1"/>
-    <col min="36" max="16384" width="9.140625" style="1"/>
+    <col min="15" max="15" width="16.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="22.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="23.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="21" style="1" customWidth="1"/>
+    <col min="22" max="22" width="24" style="1" customWidth="1"/>
+    <col min="23" max="23" width="20" style="1" customWidth="1"/>
+    <col min="24" max="25" width="17.42578125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="24" style="1" customWidth="1"/>
+    <col min="27" max="28" width="21.5703125" style="1" customWidth="1"/>
+    <col min="29" max="30" width="19.140625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="19.42578125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="19.5703125" style="1" customWidth="1"/>
+    <col min="33" max="34" width="19.140625" style="1" customWidth="1"/>
+    <col min="35" max="35" width="17" style="1" customWidth="1"/>
+    <col min="36" max="37" width="15.7109375" style="1" customWidth="1"/>
+    <col min="38" max="38" width="14.42578125" style="1" customWidth="1"/>
+    <col min="39" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>103</v>
       </c>
@@ -1880,12 +1903,15 @@
       <c r="AG1" s="27"/>
       <c r="AH1" s="27"/>
       <c r="AI1" s="27"/>
-    </row>
-    <row r="2" spans="1:35" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="27"/>
+    </row>
+    <row r="2" spans="1:38" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
       <c r="B2" s="23"/>
     </row>
-    <row r="3" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1929,70 +1955,79 @@
         <v>6</v>
       </c>
       <c r="O3" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="R3" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="R3" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="S3" s="18" t="s">
+      <c r="T3" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="U3" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="V3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="W3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="V3" s="7" t="s">
+      <c r="X3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="Y3" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="Z3" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="AA3" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="AB3" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="AA3" s="7" t="s">
+      <c r="AC3" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="AB3" s="7" t="s">
+      <c r="AD3" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="AC3" s="7" t="s">
+      <c r="AE3" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="AD3" s="7" t="s">
+      <c r="AF3" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="AE3" s="7" t="s">
+      <c r="AG3" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="AF3" s="7" t="s">
+      <c r="AH3" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="AG3" s="7" t="s">
+      <c r="AI3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AH3" s="7" t="s">
+      <c r="AJ3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AI3" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK3" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="AL3" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2015,17 +2050,17 @@
       <c r="N4" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="11"/>
+      <c r="P4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="S4" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
       <c r="V4" s="11"/>
@@ -2042,8 +2077,11 @@
       <c r="AG4" s="11"/>
       <c r="AH4" s="11"/>
       <c r="AI4" s="11"/>
-    </row>
-    <row r="5" spans="1:35" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="AJ4" s="11"/>
+      <c r="AK4" s="11"/>
+      <c r="AL4" s="11"/>
+    </row>
+    <row r="5" spans="1:38" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2062,24 +2100,24 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="15"/>
+      <c r="P5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="15" t="s">
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="Q5" s="15" t="s">
+      <c r="S5" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="R5" s="15"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
+      <c r="T5" s="15"/>
       <c r="U5" s="11"/>
       <c r="V5" s="11"/>
       <c r="W5" s="11"/>
-      <c r="X5" s="15"/>
+      <c r="X5" s="11"/>
       <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
+      <c r="Z5" s="15"/>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11"/>
       <c r="AC5" s="11"/>
@@ -2089,8 +2127,11 @@
       <c r="AG5" s="11"/>
       <c r="AH5" s="11"/>
       <c r="AI5" s="11"/>
-    </row>
-    <row r="6" spans="1:35" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ5" s="11"/>
+      <c r="AK5" s="11"/>
+      <c r="AL5" s="11"/>
+    </row>
+    <row r="6" spans="1:38" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2109,35 +2150,38 @@
         <v>221</v>
       </c>
       <c r="N6" s="11"/>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="15"/>
+      <c r="P6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="S6" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="R6" s="15"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
+      <c r="T6" s="15"/>
       <c r="U6" s="11"/>
       <c r="V6" s="11"/>
-      <c r="W6" s="15"/>
+      <c r="W6" s="11"/>
       <c r="X6" s="11"/>
       <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
+      <c r="Z6" s="11"/>
       <c r="AA6" s="15"/>
       <c r="AB6" s="15"/>
       <c r="AC6" s="15"/>
       <c r="AD6" s="15"/>
       <c r="AE6" s="15"/>
       <c r="AF6" s="15"/>
-      <c r="AG6" s="11"/>
-      <c r="AH6" s="11"/>
+      <c r="AG6" s="15"/>
+      <c r="AH6" s="15"/>
       <c r="AI6" s="11"/>
-    </row>
-    <row r="7" spans="1:35" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="AJ6" s="11"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="11"/>
+    </row>
+    <row r="7" spans="1:38" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2156,24 +2200,24 @@
         <v>215</v>
       </c>
       <c r="N7" s="11"/>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="15"/>
+      <c r="P7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="Q7" s="15" t="s">
+      <c r="S7" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="R7" s="15"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
+      <c r="T7" s="15"/>
       <c r="U7" s="11"/>
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
-      <c r="X7" s="15"/>
+      <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
+      <c r="Z7" s="15"/>
       <c r="AA7" s="11"/>
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
@@ -2183,8 +2227,11 @@
       <c r="AG7" s="11"/>
       <c r="AH7" s="11"/>
       <c r="AI7" s="11"/>
-    </row>
-    <row r="8" spans="1:35" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="AJ7" s="11"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="11"/>
+    </row>
+    <row r="8" spans="1:38" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>8</v>
       </c>
@@ -2205,21 +2252,21 @@
       <c r="N8" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="O8" s="15" t="s">
+      <c r="O8" s="15"/>
+      <c r="P8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="15" t="s">
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="Q8" s="15" t="s">
+      <c r="S8" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="R8" s="15"/>
-      <c r="S8" s="11"/>
       <c r="T8" s="15"/>
       <c r="U8" s="11"/>
       <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
+      <c r="W8" s="11"/>
       <c r="X8" s="15"/>
       <c r="Y8" s="15"/>
       <c r="Z8" s="15"/>
@@ -2229,11 +2276,14 @@
       <c r="AD8" s="15"/>
       <c r="AE8" s="15"/>
       <c r="AF8" s="15"/>
-      <c r="AG8" s="11"/>
-      <c r="AH8" s="11"/>
+      <c r="AG8" s="15"/>
+      <c r="AH8" s="15"/>
       <c r="AI8" s="11"/>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ8" s="11"/>
+      <c r="AK8" s="11"/>
+      <c r="AL8" s="11"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -2249,30 +2299,45 @@
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
+      <c r="N9" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="P9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="15" t="s">
+        <v>11</v>
+      </c>
       <c r="R9" s="15"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="U9" s="11"/>
       <c r="V9" s="11"/>
       <c r="W9" s="15"/>
       <c r="X9" s="11"/>
       <c r="Y9" s="15"/>
       <c r="Z9" s="11"/>
       <c r="AA9" s="15"/>
-      <c r="AB9" s="15"/>
+      <c r="AB9" s="11"/>
       <c r="AC9" s="15"/>
       <c r="AD9" s="15"/>
       <c r="AE9" s="15"/>
       <c r="AF9" s="15"/>
       <c r="AG9" s="15"/>
-      <c r="AH9" s="11"/>
-      <c r="AI9" s="11"/>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH9" s="15"/>
+      <c r="AI9" s="15"/>
+      <c r="AJ9" s="11"/>
+      <c r="AK9" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="AL9" s="11"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -2293,11 +2358,11 @@
       <c r="P10" s="15"/>
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="6"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
       <c r="U10" s="11"/>
       <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
+      <c r="W10" s="11"/>
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
@@ -2307,11 +2372,14 @@
       <c r="AD10" s="6"/>
       <c r="AE10" s="6"/>
       <c r="AF10" s="6"/>
-      <c r="AG10" s="11"/>
-      <c r="AH10" s="11"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="6"/>
       <c r="AI10" s="11"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ10" s="11"/>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="11"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -2332,8 +2400,8 @@
       <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
@@ -2346,11 +2414,14 @@
       <c r="AD11" s="6"/>
       <c r="AE11" s="6"/>
       <c r="AF11" s="6"/>
-      <c r="AG11" s="11"/>
-      <c r="AH11" s="11"/>
+      <c r="AG11" s="6"/>
+      <c r="AH11" s="6"/>
       <c r="AI11" s="11"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ11" s="11"/>
+      <c r="AK11" s="11"/>
+      <c r="AL11" s="11"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -2371,8 +2442,8 @@
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
@@ -2385,11 +2456,14 @@
       <c r="AD12" s="6"/>
       <c r="AE12" s="6"/>
       <c r="AF12" s="6"/>
-      <c r="AG12" s="11"/>
-      <c r="AH12" s="11"/>
+      <c r="AG12" s="6"/>
+      <c r="AH12" s="6"/>
       <c r="AI12" s="11"/>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ12" s="11"/>
+      <c r="AK12" s="11"/>
+      <c r="AL12" s="11"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
@@ -2410,8 +2484,8 @@
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
@@ -2424,11 +2498,14 @@
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
       <c r="AF13" s="6"/>
-      <c r="AG13" s="11"/>
-      <c r="AH13" s="11"/>
+      <c r="AG13" s="6"/>
+      <c r="AH13" s="6"/>
       <c r="AI13" s="11"/>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="11"/>
+      <c r="AL13" s="11"/>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -2449,8 +2526,8 @@
       <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="15"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
@@ -2463,11 +2540,14 @@
       <c r="AD14" s="6"/>
       <c r="AE14" s="6"/>
       <c r="AF14" s="6"/>
-      <c r="AG14" s="11"/>
-      <c r="AH14" s="11"/>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="6"/>
       <c r="AI14" s="11"/>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="11"/>
+      <c r="AL14" s="11"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -2488,12 +2568,12 @@
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
       <c r="R15" s="15"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
-      <c r="W15" s="19"/>
-      <c r="X15" s="19"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
       <c r="Y15" s="19"/>
       <c r="Z15" s="19"/>
       <c r="AA15" s="19"/>
@@ -2502,11 +2582,14 @@
       <c r="AD15" s="19"/>
       <c r="AE15" s="19"/>
       <c r="AF15" s="19"/>
-      <c r="AG15" s="15"/>
-      <c r="AH15" s="11"/>
-      <c r="AI15" s="11"/>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AG15" s="19"/>
+      <c r="AH15" s="19"/>
+      <c r="AI15" s="15"/>
+      <c r="AJ15" s="11"/>
+      <c r="AK15" s="11"/>
+      <c r="AL15" s="11"/>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -2527,8 +2610,8 @@
       <c r="P16" s="15"/>
       <c r="Q16" s="15"/>
       <c r="R16" s="15"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
@@ -2541,11 +2624,14 @@
       <c r="AD16" s="6"/>
       <c r="AE16" s="6"/>
       <c r="AF16" s="6"/>
-      <c r="AG16" s="11"/>
-      <c r="AH16" s="11"/>
+      <c r="AG16" s="6"/>
+      <c r="AH16" s="6"/>
       <c r="AI16" s="11"/>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ16" s="11"/>
+      <c r="AK16" s="11"/>
+      <c r="AL16" s="11"/>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>30</v>
       </c>
@@ -2562,12 +2648,12 @@
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="15"/>
+      <c r="O17" s="19"/>
       <c r="P17" s="15"/>
       <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
@@ -2582,9 +2668,12 @@
       <c r="AF17" s="6"/>
       <c r="AG17" s="6"/>
       <c r="AH17" s="6"/>
-      <c r="AI17" s="11"/>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AI17" s="6"/>
+      <c r="AJ17" s="6"/>
+      <c r="AK17" s="6"/>
+      <c r="AL17" s="11"/>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
@@ -2601,12 +2690,12 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
-      <c r="O18" s="15"/>
+      <c r="O18" s="19"/>
       <c r="P18" s="15"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
@@ -2621,10 +2710,13 @@
       <c r="AF18" s="6"/>
       <c r="AG18" s="6"/>
       <c r="AH18" s="6"/>
-      <c r="AI18" s="11"/>
+      <c r="AI18" s="6"/>
       <c r="AJ18" s="6"/>
-    </row>
-    <row r="19" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK18" s="6"/>
+      <c r="AL18" s="11"/>
+      <c r="AM18" s="6"/>
+    </row>
+    <row r="19" spans="1:39" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>73</v>
       </c>
@@ -2662,8 +2754,11 @@
       <c r="AG19" s="11"/>
       <c r="AH19" s="11"/>
       <c r="AI19" s="11"/>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ19" s="11"/>
+      <c r="AK19" s="11"/>
+      <c r="AL19" s="11"/>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>74</v>
       </c>
@@ -2684,12 +2779,12 @@
       <c r="P20" s="15"/>
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
-      <c r="W20" s="19"/>
-      <c r="X20" s="19"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
       <c r="Y20" s="19"/>
       <c r="Z20" s="19"/>
       <c r="AA20" s="19"/>
@@ -2698,14 +2793,17 @@
       <c r="AD20" s="19"/>
       <c r="AE20" s="19"/>
       <c r="AF20" s="19"/>
-      <c r="AG20" s="15"/>
-      <c r="AH20" s="11"/>
-      <c r="AI20" s="11"/>
+      <c r="AG20" s="19"/>
+      <c r="AH20" s="19"/>
+      <c r="AI20" s="15"/>
+      <c r="AJ20" s="11"/>
+      <c r="AK20" s="11"/>
+      <c r="AL20" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:AI1"/>
+    <mergeCell ref="A1:AL1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3707,7 +3805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D05107-472F-4DD1-88F8-DE97CAF36E00}">
   <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>

</xml_diff>